<commit_message>
[LPF-868]: Mediation contract balances - update template
Signed-off-by: robert.buczek <robert.buczek@digital.justice.gov.uk>
</commit_message>
<xml_diff>
--- a/src/main/resources/MEDIATION_CONTRACT_BALANCES_TEMPLATE.xlsx
+++ b/src/main/resources/MEDIATION_CONTRACT_BALANCES_TEMPLATE.xlsx
@@ -9,7 +9,6 @@
     <sheet name="MAIN" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Adjusted Expenditure" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Files to import" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'MAIN'!$C$5:$E$7</definedName>
@@ -1090,7 +1089,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1123,38 +1122,429 @@
       <c r="E1" s="2" t="n"/>
       <c r="F1" s="2" t="n"/>
     </row>
-    <row r="2" ht="15" customHeight="1"/>
-    <row r="3" ht="15" customHeight="1"/>
-    <row r="4" ht="15" customHeight="1"/>
-    <row r="5" ht="15" customHeight="1"/>
-    <row r="6" ht="15" customHeight="1"/>
-    <row r="7" ht="39" customHeight="1"/>
-    <row r="8" ht="15" customHeight="1"/>
-    <row r="9" ht="15" customHeight="1"/>
-    <row r="10" ht="15" customHeight="1"/>
-    <row r="11" ht="15" customHeight="1"/>
-    <row r="12" ht="15" customHeight="1"/>
-    <row r="13" ht="15" customHeight="1"/>
-    <row r="14" ht="15" customHeight="1"/>
-    <row r="15" ht="15" customHeight="1"/>
-    <row r="16" ht="15" customHeight="1"/>
-    <row r="17" ht="15" customHeight="1"/>
-    <row r="18" ht="15" customHeight="1"/>
-    <row r="19" ht="15" customHeight="1"/>
-    <row r="20" ht="15" customHeight="1"/>
-    <row r="21" ht="15" customHeight="1"/>
-    <row r="22" ht="15" customHeight="1"/>
-    <row r="23" ht="15" customHeight="1"/>
-    <row r="24" ht="15" customHeight="1"/>
-    <row r="25" ht="15" customHeight="1"/>
-    <row r="26" ht="15" customHeight="1"/>
-    <row r="27" ht="15" customHeight="1" thickBot="1"/>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="9" t="n"/>
+      <c r="B2" s="20" t="n"/>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="10" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Data extraction </t>
+        </is>
+      </c>
+      <c r="B3" s="21" t="n"/>
+      <c r="C3" s="6" t="n"/>
+      <c r="D3" s="10" t="n"/>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="18" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="9" t="n"/>
+      <c r="B4" s="20" t="n"/>
+      <c r="C4" s="4" t="n"/>
+      <c r="D4" s="10" t="n"/>
+      <c r="F4" s="2" t="n"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="20" t="n"/>
+      <c r="B5" s="20" t="n"/>
+      <c r="C5" s="17" t="n"/>
+      <c r="D5" s="12" t="n"/>
+      <c r="F5" s="2" t="n"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="20" t="n"/>
+      <c r="B6" s="20" t="n"/>
+      <c r="C6" s="17" t="n"/>
+      <c r="D6" s="12" t="n"/>
+      <c r="F6" s="2" t="n"/>
+    </row>
+    <row r="7" ht="39" customHeight="1">
+      <c r="A7" s="13" t="n"/>
+      <c r="B7" s="22" t="n"/>
+      <c r="C7" s="14" t="n"/>
+      <c r="D7" s="15" t="n"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="D8" s="2" t="n"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Claims</t>
+        </is>
+      </c>
+      <c r="B9" s="18" t="inlineStr">
+        <is>
+          <t>All suppliers</t>
+        </is>
+      </c>
+      <c r="C9" s="25" t="n"/>
+      <c r="D9" s="23" t="inlineStr">
+        <is>
+          <t>Balanced suppliers</t>
+        </is>
+      </c>
+      <c r="E9" s="18" t="inlineStr">
+        <is>
+          <t>Over paid suppliers</t>
+        </is>
+      </c>
+      <c r="F9" s="18" t="inlineStr">
+        <is>
+          <t>Under paid</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Older than 12 months</t>
+        </is>
+      </c>
+      <c r="B10" s="2">
+        <f>SUM(DATA!B:B)</f>
+        <v/>
+      </c>
+      <c r="D10" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$B:$B)</f>
+        <v/>
+      </c>
+      <c r="E10" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$B:$B)</f>
+        <v/>
+      </c>
+      <c r="F10" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$B:$B)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>In last 12 months</t>
+        </is>
+      </c>
+      <c r="B11" s="2">
+        <f>SUM(DATA!C:C)</f>
+        <v/>
+      </c>
+      <c r="D11" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$C:$C)</f>
+        <v/>
+      </c>
+      <c r="E11" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$C:$C)</f>
+        <v/>
+      </c>
+      <c r="F11" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$C:$C)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1">
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="2" t="n"/>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>A) Total claims</t>
+        </is>
+      </c>
+      <c r="B13" s="2">
+        <f>B10+B11</f>
+        <v/>
+      </c>
+      <c r="D13" s="2">
+        <f>SUM(D10:D12)</f>
+        <v/>
+      </c>
+      <c r="E13" s="2">
+        <f>SUM(E10:E12)</f>
+        <v/>
+      </c>
+      <c r="F13" s="2">
+        <f>SUM(F10:F12)</f>
+        <v/>
+      </c>
+      <c r="I13" s="33" t="n"/>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="B14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="2" t="n"/>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Contract payments and expenditure</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
+    </row>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Older than 12 months</t>
+        </is>
+      </c>
+      <c r="B16" s="2">
+        <f>SUM(DATA!E:E)</f>
+        <v/>
+      </c>
+      <c r="D16" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$E:$E)</f>
+        <v/>
+      </c>
+      <c r="E16" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$E:$E)</f>
+        <v/>
+      </c>
+      <c r="F16" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$E:$E)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>In last 12 months</t>
+        </is>
+      </c>
+      <c r="B17" s="2">
+        <f>SUM(DATA!F:F)</f>
+        <v/>
+      </c>
+      <c r="D17" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$F:$F)</f>
+        <v/>
+      </c>
+      <c r="E17" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$F:$F)</f>
+        <v/>
+      </c>
+      <c r="F17" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$F:$F)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Adjustment due to missing  payments</t>
+        </is>
+      </c>
+      <c r="B18" s="2">
+        <f>SUM(DATA!M:M)</f>
+        <v/>
+      </c>
+      <c r="D18" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$M:$M)</f>
+        <v/>
+      </c>
+      <c r="E18" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$M:$M)</f>
+        <v/>
+      </c>
+      <c r="F18" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$M:$M)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1">
+      <c r="B19" s="2" t="n"/>
+      <c r="D19" s="2" t="n"/>
+      <c r="E19" s="2" t="n"/>
+      <c r="F19" s="2" t="n"/>
+    </row>
+    <row r="20" ht="15" customHeight="1">
+      <c r="B20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
+      <c r="F20" s="2" t="n"/>
+    </row>
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>B) Total expenditure</t>
+        </is>
+      </c>
+      <c r="B21" s="2">
+        <f>B16+B17+B18</f>
+        <v/>
+      </c>
+      <c r="D21" s="2">
+        <f>D16+D17+D18</f>
+        <v/>
+      </c>
+      <c r="E21" s="2">
+        <f>E16+E17+E18</f>
+        <v/>
+      </c>
+      <c r="F21" s="2">
+        <f>F16+F17+F18</f>
+        <v/>
+      </c>
+      <c r="I21" s="33" t="n"/>
+    </row>
+    <row r="22" ht="15" customHeight="1">
+      <c r="B22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
+      <c r="E22" s="2" t="n"/>
+      <c r="F22" s="2" t="n"/>
+    </row>
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" s="26" t="inlineStr">
+        <is>
+          <t>C) Balance of claims and payments (A - B)</t>
+        </is>
+      </c>
+      <c r="B23" s="27">
+        <f>B13-B21</f>
+        <v/>
+      </c>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="27">
+        <f>D13-D21</f>
+        <v/>
+      </c>
+      <c r="E23" s="27">
+        <f>E13-E21</f>
+        <v/>
+      </c>
+      <c r="F23" s="27">
+        <f>F13-F21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="D24" s="2" t="n"/>
+      <c r="E24" s="2" t="n"/>
+      <c r="F24" s="2" t="n"/>
+    </row>
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>D) Total contract adjustments</t>
+        </is>
+      </c>
+      <c r="B25" s="2">
+        <f>SUM(DATA!I:I)</f>
+        <v/>
+      </c>
+      <c r="D25" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$I:$I)</f>
+        <v/>
+      </c>
+      <c r="E25" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$I:$I)</f>
+        <v/>
+      </c>
+      <c r="F25" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$I:$I)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1">
+      <c r="D26" s="2" t="n"/>
+      <c r="E26" s="2" t="n"/>
+      <c r="F26" s="2" t="n"/>
+    </row>
+    <row r="27" ht="15" customHeight="1" thickBot="1">
+      <c r="A27" s="28" t="inlineStr">
+        <is>
+          <t>E) Contract balance (C + D)</t>
+        </is>
+      </c>
+      <c r="B27" s="29">
+        <f>B23+B25</f>
+        <v/>
+      </c>
+      <c r="C27" s="1" t="n"/>
+      <c r="D27" s="29">
+        <f>D23+D25</f>
+        <v/>
+      </c>
+      <c r="E27" s="29">
+        <f>E23+E25</f>
+        <v/>
+      </c>
+      <c r="F27" s="29">
+        <f>F23+F25</f>
+        <v/>
+      </c>
+    </row>
     <row r="28" ht="15" customHeight="1" thickTop="1"/>
-    <row r="29" ht="15" customHeight="1"/>
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Checksum</t>
+        </is>
+      </c>
+      <c r="B29" s="2">
+        <f>SUM(DATA!N:N)-B27</f>
+        <v/>
+      </c>
+      <c r="D29" s="25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E29" s="2">
+        <f>SUMIF(DATA!N:N,"&lt;0",DATA!N:N)-E27</f>
+        <v/>
+      </c>
+      <c r="F29" s="2">
+        <f>SUMIF(DATA!N:N,"&gt;0",DATA!N:N)-F27</f>
+        <v/>
+      </c>
+    </row>
     <row r="30" ht="15" customHeight="1"/>
-    <row r="31" ht="15" customHeight="1"/>
-    <row r="32" ht="15" customHeight="1"/>
-    <row r="33" ht="15" customHeight="1"/>
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Payments in year</t>
+        </is>
+      </c>
+      <c r="B31" s="30">
+        <f>SUM(DATA!L:L)+SUM(DATA!M:M)</f>
+        <v/>
+      </c>
+      <c r="C31" s="2" t="n"/>
+      <c r="D31" s="31" t="n"/>
+      <c r="E31" s="18" t="n"/>
+      <c r="F31" s="18" t="n"/>
+    </row>
+    <row r="32" ht="15" customHeight="1">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>In year contract payments (Bank report) (Not including pre Apr-2015 scheme payments &amp; claims)</t>
+        </is>
+      </c>
+      <c r="B32" s="30" t="n"/>
+      <c r="C32" s="3" t="n"/>
+      <c r="D32" s="2" t="n"/>
+      <c r="E32" s="2" t="n"/>
+      <c r="F32" s="2" t="n"/>
+    </row>
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>SIMPLE CHECK</t>
+        </is>
+      </c>
+      <c r="B33" s="2">
+        <f>475000*9</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.7480314960629921" bottom="0.1574803149606299" header="0.3149606299212598" footer="0.3149606299212598"/>
   <pageSetup orientation="portrait" paperSize="9" scale="92"/>
@@ -1326,52 +1716,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet4">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A3:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="36.85546875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="113.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="50.140625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="32" t="inlineStr">
-        <is>
-          <t>Target sheet name</t>
-        </is>
-      </c>
-      <c r="B1" s="32" t="inlineStr">
-        <is>
-          <t>Source folder</t>
-        </is>
-      </c>
-      <c r="C1" s="32" t="inlineStr">
-        <is>
-          <t>Source file name</t>
-        </is>
-      </c>
-      <c r="D1" s="32" t="inlineStr">
-        <is>
-          <t>Sheet number</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[LPF-868]: Mediation contract balances - update template (#247)
Signed-off-by: robert.buczek <robert.buczek@digital.justice.gov.uk>
</commit_message>
<xml_diff>
--- a/src/main/resources/MEDIATION_CONTRACT_BALANCES_TEMPLATE.xlsx
+++ b/src/main/resources/MEDIATION_CONTRACT_BALANCES_TEMPLATE.xlsx
@@ -9,7 +9,6 @@
     <sheet name="MAIN" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Adjusted Expenditure" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Files to import" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'MAIN'!$C$5:$E$7</definedName>
@@ -1090,7 +1089,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1123,38 +1122,429 @@
       <c r="E1" s="2" t="n"/>
       <c r="F1" s="2" t="n"/>
     </row>
-    <row r="2" ht="15" customHeight="1"/>
-    <row r="3" ht="15" customHeight="1"/>
-    <row r="4" ht="15" customHeight="1"/>
-    <row r="5" ht="15" customHeight="1"/>
-    <row r="6" ht="15" customHeight="1"/>
-    <row r="7" ht="39" customHeight="1"/>
-    <row r="8" ht="15" customHeight="1"/>
-    <row r="9" ht="15" customHeight="1"/>
-    <row r="10" ht="15" customHeight="1"/>
-    <row r="11" ht="15" customHeight="1"/>
-    <row r="12" ht="15" customHeight="1"/>
-    <row r="13" ht="15" customHeight="1"/>
-    <row r="14" ht="15" customHeight="1"/>
-    <row r="15" ht="15" customHeight="1"/>
-    <row r="16" ht="15" customHeight="1"/>
-    <row r="17" ht="15" customHeight="1"/>
-    <row r="18" ht="15" customHeight="1"/>
-    <row r="19" ht="15" customHeight="1"/>
-    <row r="20" ht="15" customHeight="1"/>
-    <row r="21" ht="15" customHeight="1"/>
-    <row r="22" ht="15" customHeight="1"/>
-    <row r="23" ht="15" customHeight="1"/>
-    <row r="24" ht="15" customHeight="1"/>
-    <row r="25" ht="15" customHeight="1"/>
-    <row r="26" ht="15" customHeight="1"/>
-    <row r="27" ht="15" customHeight="1" thickBot="1"/>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="9" t="n"/>
+      <c r="B2" s="20" t="n"/>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="10" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Data extraction </t>
+        </is>
+      </c>
+      <c r="B3" s="21" t="n"/>
+      <c r="C3" s="6" t="n"/>
+      <c r="D3" s="10" t="n"/>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="18" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="9" t="n"/>
+      <c r="B4" s="20" t="n"/>
+      <c r="C4" s="4" t="n"/>
+      <c r="D4" s="10" t="n"/>
+      <c r="F4" s="2" t="n"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="20" t="n"/>
+      <c r="B5" s="20" t="n"/>
+      <c r="C5" s="17" t="n"/>
+      <c r="D5" s="12" t="n"/>
+      <c r="F5" s="2" t="n"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="20" t="n"/>
+      <c r="B6" s="20" t="n"/>
+      <c r="C6" s="17" t="n"/>
+      <c r="D6" s="12" t="n"/>
+      <c r="F6" s="2" t="n"/>
+    </row>
+    <row r="7" ht="39" customHeight="1">
+      <c r="A7" s="13" t="n"/>
+      <c r="B7" s="22" t="n"/>
+      <c r="C7" s="14" t="n"/>
+      <c r="D7" s="15" t="n"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="D8" s="2" t="n"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Claims</t>
+        </is>
+      </c>
+      <c r="B9" s="18" t="inlineStr">
+        <is>
+          <t>All suppliers</t>
+        </is>
+      </c>
+      <c r="C9" s="25" t="n"/>
+      <c r="D9" s="23" t="inlineStr">
+        <is>
+          <t>Balanced suppliers</t>
+        </is>
+      </c>
+      <c r="E9" s="18" t="inlineStr">
+        <is>
+          <t>Over paid suppliers</t>
+        </is>
+      </c>
+      <c r="F9" s="18" t="inlineStr">
+        <is>
+          <t>Under paid</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Older than 12 months</t>
+        </is>
+      </c>
+      <c r="B10" s="2">
+        <f>SUM(DATA!B:B)</f>
+        <v/>
+      </c>
+      <c r="D10" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$B:$B)</f>
+        <v/>
+      </c>
+      <c r="E10" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$B:$B)</f>
+        <v/>
+      </c>
+      <c r="F10" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$B:$B)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>In last 12 months</t>
+        </is>
+      </c>
+      <c r="B11" s="2">
+        <f>SUM(DATA!C:C)</f>
+        <v/>
+      </c>
+      <c r="D11" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$C:$C)</f>
+        <v/>
+      </c>
+      <c r="E11" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$C:$C)</f>
+        <v/>
+      </c>
+      <c r="F11" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$C:$C)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1">
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="2" t="n"/>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>A) Total claims</t>
+        </is>
+      </c>
+      <c r="B13" s="2">
+        <f>B10+B11</f>
+        <v/>
+      </c>
+      <c r="D13" s="2">
+        <f>SUM(D10:D12)</f>
+        <v/>
+      </c>
+      <c r="E13" s="2">
+        <f>SUM(E10:E12)</f>
+        <v/>
+      </c>
+      <c r="F13" s="2">
+        <f>SUM(F10:F12)</f>
+        <v/>
+      </c>
+      <c r="I13" s="33" t="n"/>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="B14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="2" t="n"/>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Contract payments and expenditure</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
+    </row>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Older than 12 months</t>
+        </is>
+      </c>
+      <c r="B16" s="2">
+        <f>SUM(DATA!E:E)</f>
+        <v/>
+      </c>
+      <c r="D16" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$E:$E)</f>
+        <v/>
+      </c>
+      <c r="E16" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$E:$E)</f>
+        <v/>
+      </c>
+      <c r="F16" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$E:$E)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>In last 12 months</t>
+        </is>
+      </c>
+      <c r="B17" s="2">
+        <f>SUM(DATA!F:F)</f>
+        <v/>
+      </c>
+      <c r="D17" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$F:$F)</f>
+        <v/>
+      </c>
+      <c r="E17" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$F:$F)</f>
+        <v/>
+      </c>
+      <c r="F17" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$F:$F)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Adjustment due to missing  payments</t>
+        </is>
+      </c>
+      <c r="B18" s="2">
+        <f>SUM(DATA!M:M)</f>
+        <v/>
+      </c>
+      <c r="D18" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$M:$M)</f>
+        <v/>
+      </c>
+      <c r="E18" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$M:$M)</f>
+        <v/>
+      </c>
+      <c r="F18" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$M:$M)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1">
+      <c r="B19" s="2" t="n"/>
+      <c r="D19" s="2" t="n"/>
+      <c r="E19" s="2" t="n"/>
+      <c r="F19" s="2" t="n"/>
+    </row>
+    <row r="20" ht="15" customHeight="1">
+      <c r="B20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
+      <c r="F20" s="2" t="n"/>
+    </row>
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>B) Total expenditure</t>
+        </is>
+      </c>
+      <c r="B21" s="2">
+        <f>B16+B17+B18</f>
+        <v/>
+      </c>
+      <c r="D21" s="2">
+        <f>D16+D17+D18</f>
+        <v/>
+      </c>
+      <c r="E21" s="2">
+        <f>E16+E17+E18</f>
+        <v/>
+      </c>
+      <c r="F21" s="2">
+        <f>F16+F17+F18</f>
+        <v/>
+      </c>
+      <c r="I21" s="33" t="n"/>
+    </row>
+    <row r="22" ht="15" customHeight="1">
+      <c r="B22" s="2" t="n"/>
+      <c r="D22" s="2" t="n"/>
+      <c r="E22" s="2" t="n"/>
+      <c r="F22" s="2" t="n"/>
+    </row>
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" s="26" t="inlineStr">
+        <is>
+          <t>C) Balance of claims and payments (A - B)</t>
+        </is>
+      </c>
+      <c r="B23" s="27">
+        <f>B13-B21</f>
+        <v/>
+      </c>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="27">
+        <f>D13-D21</f>
+        <v/>
+      </c>
+      <c r="E23" s="27">
+        <f>E13-E21</f>
+        <v/>
+      </c>
+      <c r="F23" s="27">
+        <f>F13-F21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="D24" s="2" t="n"/>
+      <c r="E24" s="2" t="n"/>
+      <c r="F24" s="2" t="n"/>
+    </row>
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>D) Total contract adjustments</t>
+        </is>
+      </c>
+      <c r="B25" s="2">
+        <f>SUM(DATA!I:I)</f>
+        <v/>
+      </c>
+      <c r="D25" s="2">
+        <f>SUMIF(DATA!$N:$N,0,DATA!$I:$I)</f>
+        <v/>
+      </c>
+      <c r="E25" s="2">
+        <f>SUMIF(DATA!$N:$N,"&lt;0",DATA!$I:$I)</f>
+        <v/>
+      </c>
+      <c r="F25" s="2">
+        <f>SUMIF(DATA!$N:$N,"&gt;0",DATA!$I:$I)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1">
+      <c r="D26" s="2" t="n"/>
+      <c r="E26" s="2" t="n"/>
+      <c r="F26" s="2" t="n"/>
+    </row>
+    <row r="27" ht="15" customHeight="1" thickBot="1">
+      <c r="A27" s="28" t="inlineStr">
+        <is>
+          <t>E) Contract balance (C + D)</t>
+        </is>
+      </c>
+      <c r="B27" s="29">
+        <f>B23+B25</f>
+        <v/>
+      </c>
+      <c r="C27" s="1" t="n"/>
+      <c r="D27" s="29">
+        <f>D23+D25</f>
+        <v/>
+      </c>
+      <c r="E27" s="29">
+        <f>E23+E25</f>
+        <v/>
+      </c>
+      <c r="F27" s="29">
+        <f>F23+F25</f>
+        <v/>
+      </c>
+    </row>
     <row r="28" ht="15" customHeight="1" thickTop="1"/>
-    <row r="29" ht="15" customHeight="1"/>
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Checksum</t>
+        </is>
+      </c>
+      <c r="B29" s="2">
+        <f>SUM(DATA!N:N)-B27</f>
+        <v/>
+      </c>
+      <c r="D29" s="25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E29" s="2">
+        <f>SUMIF(DATA!N:N,"&lt;0",DATA!N:N)-E27</f>
+        <v/>
+      </c>
+      <c r="F29" s="2">
+        <f>SUMIF(DATA!N:N,"&gt;0",DATA!N:N)-F27</f>
+        <v/>
+      </c>
+    </row>
     <row r="30" ht="15" customHeight="1"/>
-    <row r="31" ht="15" customHeight="1"/>
-    <row r="32" ht="15" customHeight="1"/>
-    <row r="33" ht="15" customHeight="1"/>
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Payments in year</t>
+        </is>
+      </c>
+      <c r="B31" s="30">
+        <f>SUM(DATA!L:L)+SUM(DATA!M:M)</f>
+        <v/>
+      </c>
+      <c r="C31" s="2" t="n"/>
+      <c r="D31" s="31" t="n"/>
+      <c r="E31" s="18" t="n"/>
+      <c r="F31" s="18" t="n"/>
+    </row>
+    <row r="32" ht="15" customHeight="1">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>In year contract payments (Bank report) (Not including pre Apr-2015 scheme payments &amp; claims)</t>
+        </is>
+      </c>
+      <c r="B32" s="30" t="n"/>
+      <c r="C32" s="3" t="n"/>
+      <c r="D32" s="2" t="n"/>
+      <c r="E32" s="2" t="n"/>
+      <c r="F32" s="2" t="n"/>
+    </row>
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>SIMPLE CHECK</t>
+        </is>
+      </c>
+      <c r="B33" s="2">
+        <f>475000*9</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.7480314960629921" bottom="0.1574803149606299" header="0.3149606299212598" footer="0.3149606299212598"/>
   <pageSetup orientation="portrait" paperSize="9" scale="92"/>
@@ -1326,52 +1716,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet4">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A3:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="36.85546875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="113.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="50.140625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="32" t="inlineStr">
-        <is>
-          <t>Target sheet name</t>
-        </is>
-      </c>
-      <c r="B1" s="32" t="inlineStr">
-        <is>
-          <t>Source folder</t>
-        </is>
-      </c>
-      <c r="C1" s="32" t="inlineStr">
-        <is>
-          <t>Source file name</t>
-        </is>
-      </c>
-      <c r="D1" s="32" t="inlineStr">
-        <is>
-          <t>Sheet number</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
-</worksheet>
 </file>
</xml_diff>